<commit_message>
Update 2022 site coordinates
</commit_message>
<xml_diff>
--- a/data/subcatchments_metadata/tana_2022_sensor_sites_outlet_coords.xlsx
+++ b/data/subcatchments_metadata/tana_2022_sensor_sites_outlet_coords.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\GitHub\quantom\data\subcatchments_metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F95D4DC3-BFD3-46FF-A352-0369FBF5F3E5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7C4E023-E7B4-4E9A-B494-4071BF66DB24}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{9A1482E1-89A6-4694-9ADB-0D51ABF83602}"/>
   </bookViews>
@@ -63,9 +63,6 @@
     <t>site_name</t>
   </si>
   <si>
-    <t>M1</t>
-  </si>
-  <si>
     <t>lat</t>
   </si>
   <si>
@@ -82,6 +79,9 @@
   </si>
   <si>
     <t>Karasjohka</t>
+  </si>
+  <si>
+    <t>M0</t>
   </si>
 </sst>
 </file>
@@ -469,7 +469,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B4"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -485,15 +485,15 @@
         <v>9</v>
       </c>
       <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
         <v>11</v>
-      </c>
-      <c r="D1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -507,10 +507,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>14</v>
       </c>
       <c r="C3" s="4">
         <v>69.398449999999997</v>
@@ -521,10 +521,10 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>16</v>
       </c>
       <c r="C4" s="4">
         <v>69.397360000000006</v>

</xml_diff>